<commit_message>
this is the october month commit
</commit_message>
<xml_diff>
--- a/src/test/java/com/Pavanselframework/testdata/LoginData.xlsx
+++ b/src/test/java/com/Pavanselframework/testdata/LoginData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13815" windowHeight="5085"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13650" windowHeight="6465"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,12 +40,6 @@
     <t>tytUreg</t>
   </si>
   <si>
-    <t>mngr137319</t>
-  </si>
-  <si>
-    <t>bAdYvyb</t>
-  </si>
-  <si>
     <t>mngr332988</t>
   </si>
   <si>
@@ -56,6 +50,12 @@
   </si>
   <si>
     <t>agerUtY</t>
+  </si>
+  <si>
+    <t>mngr353217</t>
+  </si>
+  <si>
+    <t>ehadEru</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -448,7 +448,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -467,10 +467,10 @@
     </row>
     <row r="2" spans="1:2" ht="23.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="23.25">
@@ -483,18 +483,18 @@
     </row>
     <row r="4" spans="1:2" ht="23.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="23.25">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="23.25">
@@ -507,10 +507,10 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>